<commit_message>
Adding Recursive and Btree Problems
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parag jain\Desktop\DSA_CRACK_SHEET_SOLUTION_LOVE_BABBER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA45C09-C477-482B-8C5B-0A96A558D3F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0414E1D0-C10E-4F71-B9CA-32EA61E1B0CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="479">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1441,13 +1441,34 @@
   </si>
   <si>
     <t>Recursion</t>
+  </si>
+  <si>
+    <t>Problems added By Parag Jain for extra Topic Based Practice</t>
+  </si>
+  <si>
+    <t>Traverse array and print all element using recursion</t>
+  </si>
+  <si>
+    <t>Reverse print an array using recursion</t>
+  </si>
+  <si>
+    <t>Determine whether or not a string is a palindrome</t>
+  </si>
+  <si>
+    <t>Find the power of x</t>
+  </si>
+  <si>
+    <t>print-all-possible-combinations-of-r-elements-in-a-given-array-of-size-n</t>
+  </si>
+  <si>
+    <t>program-chocolate-wrapper-puzzle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1512,6 +1533,13 @@
     <font>
       <sz val="12"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1597,7 +1625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1645,6 +1673,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1962,10 +2005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:F482"/>
+  <dimension ref="A1:F490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="C185" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3313,16 +3356,18 @@
       <c r="A93" s="3">
         <v>38</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C93" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="E93" t="s">
         <v>471</v>
       </c>
-      <c r="E93"/>
     </row>
     <row r="94" spans="1:5" s="20" customFormat="1" ht="21">
       <c r="A94" s="3">
@@ -3386,13 +3431,13 @@
       <c r="A98" s="3">
         <v>43</v>
       </c>
-      <c r="B98" s="10" t="s">
+      <c r="B98" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C98" s="11" t="s">
+      <c r="C98" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D98" s="14" t="s">
+      <c r="D98" s="3" t="s">
         <v>463</v>
       </c>
       <c r="E98"/>
@@ -4449,182 +4494,210 @@
       <c r="A177" s="3">
         <v>1</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B177" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C177" s="5" t="s">
+      <c r="C177" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="D177" s="3"/>
+      <c r="D177" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E177"/>
     </row>
     <row r="178" spans="1:5" s="20" customFormat="1" ht="21">
       <c r="A178" s="3">
         <v>2</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B178" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C178" s="5" t="s">
+      <c r="C178" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D178" s="3"/>
+      <c r="D178" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E178"/>
     </row>
     <row r="179" spans="1:5" s="20" customFormat="1" ht="21">
       <c r="A179" s="3">
         <v>3</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B179" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C179" s="5" t="s">
+      <c r="C179" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="D179" s="3"/>
+      <c r="D179" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E179"/>
     </row>
     <row r="180" spans="1:5" s="20" customFormat="1" ht="21">
       <c r="A180" s="3">
         <v>4</v>
       </c>
-      <c r="B180" s="4" t="s">
+      <c r="B180" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C180" s="5" t="s">
+      <c r="C180" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="D180" s="3"/>
+      <c r="D180" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E180"/>
     </row>
     <row r="181" spans="1:5" s="20" customFormat="1" ht="21">
-      <c r="A181" s="3">
+      <c r="A181" s="21">
         <v>5</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B181" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C181" s="5" t="s">
+      <c r="C181" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="D181" s="3"/>
+      <c r="D181" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E181"/>
     </row>
     <row r="182" spans="1:5" s="20" customFormat="1" ht="21">
-      <c r="A182" s="3">
+      <c r="A182" s="22">
         <v>6</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B182" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C182" s="5" t="s">
+      <c r="C182" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="D182" s="3"/>
+      <c r="D182" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E182"/>
     </row>
     <row r="183" spans="1:5" s="20" customFormat="1" ht="21">
-      <c r="A183" s="3">
+      <c r="A183" s="22">
         <v>7</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B183" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C183" s="5" t="s">
+      <c r="C183" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D183" s="3"/>
+      <c r="D183" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E183"/>
     </row>
     <row r="184" spans="1:5" s="20" customFormat="1" ht="21">
-      <c r="A184" s="3">
+      <c r="A184" s="22">
         <v>8</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B184" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C184" s="5" t="s">
+      <c r="C184" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="D184" s="3"/>
+      <c r="D184" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E184"/>
     </row>
     <row r="185" spans="1:5" s="20" customFormat="1" ht="21">
-      <c r="A185" s="3">
+      <c r="A185" s="22">
         <v>9</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B185" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C185" s="5" t="s">
+      <c r="C185" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D185" s="3"/>
+      <c r="D185" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E185"/>
     </row>
     <row r="186" spans="1:5" s="20" customFormat="1" ht="21">
-      <c r="A186" s="3">
+      <c r="A186" s="23">
         <v>10</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="B186" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C186" s="5" t="s">
+      <c r="C186" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="D186" s="3"/>
+      <c r="D186" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E186"/>
     </row>
     <row r="187" spans="1:5" s="20" customFormat="1" ht="21">
-      <c r="A187" s="3">
+      <c r="A187" s="23">
         <v>11</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="B187" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C187" s="5" t="s">
+      <c r="C187" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="D187" s="3"/>
+      <c r="D187" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E187"/>
     </row>
     <row r="188" spans="1:5" s="20" customFormat="1" ht="21">
-      <c r="A188" s="3">
+      <c r="A188" s="23">
         <v>12</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B188" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C188" s="5" t="s">
+      <c r="C188" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="D188" s="3"/>
+      <c r="D188" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E188"/>
     </row>
     <row r="189" spans="1:5" s="20" customFormat="1" ht="21">
-      <c r="A189" s="3">
+      <c r="A189" s="23">
         <v>13</v>
       </c>
-      <c r="B189" s="4" t="s">
+      <c r="B189" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C189" s="5" t="s">
+      <c r="C189" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="D189" s="3"/>
+      <c r="D189" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E189"/>
     </row>
     <row r="190" spans="1:5" s="20" customFormat="1" ht="21">
-      <c r="A190" s="3">
+      <c r="A190" s="23">
         <v>14</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="B190" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C190" s="5" t="s">
+      <c r="C190" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="D190" s="3"/>
+      <c r="D190" s="14" t="s">
+        <v>463</v>
+      </c>
       <c r="E190"/>
     </row>
     <row r="191" spans="1:5" s="20" customFormat="1" ht="21">
@@ -8309,7 +8382,94 @@
       <c r="D482" s="3"/>
       <c r="E482"/>
     </row>
+    <row r="484" spans="1:5" ht="25.8">
+      <c r="B484" s="24" t="s">
+        <v>472</v>
+      </c>
+      <c r="C484" s="25"/>
+    </row>
+    <row r="485" spans="1:5" s="20" customFormat="1" ht="21">
+      <c r="A485" s="3">
+        <v>1</v>
+      </c>
+      <c r="B485" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C485" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="D485" s="3"/>
+      <c r="E485"/>
+    </row>
+    <row r="486" spans="1:5" s="20" customFormat="1" ht="21">
+      <c r="A486" s="3">
+        <v>2</v>
+      </c>
+      <c r="B486" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C486" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="D486" s="3"/>
+      <c r="E486"/>
+    </row>
+    <row r="487" spans="1:5" s="20" customFormat="1" ht="21">
+      <c r="A487" s="3">
+        <v>3</v>
+      </c>
+      <c r="B487" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C487" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="D487" s="3"/>
+      <c r="E487"/>
+    </row>
+    <row r="488" spans="1:5" s="20" customFormat="1" ht="21">
+      <c r="A488" s="3">
+        <v>4</v>
+      </c>
+      <c r="B488" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C488" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="D488" s="3"/>
+      <c r="E488"/>
+    </row>
+    <row r="489" spans="1:5" s="20" customFormat="1" ht="21">
+      <c r="A489" s="3">
+        <v>5</v>
+      </c>
+      <c r="B489" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C489" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="D489" s="3"/>
+      <c r="E489"/>
+    </row>
+    <row r="490" spans="1:5" s="20" customFormat="1" ht="21">
+      <c r="A490" s="3">
+        <v>6</v>
+      </c>
+      <c r="B490" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="C490" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="D490" s="3"/>
+      <c r="E490"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B484:C484"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>
     <hyperlink ref="C7" r:id="rId2" xr:uid="{2D6F1134-3C08-7445-B19A-9B94A18B55C7}"/>
@@ -8757,8 +8917,9 @@
     <hyperlink ref="C2" r:id="rId444" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
     <hyperlink ref="C66" r:id="rId445" xr:uid="{927AE532-647F-AF4C-A567-40ADA6FCE534}"/>
     <hyperlink ref="C90" r:id="rId446" xr:uid="{E6BEE510-1E91-400E-AA3E-84C4045CB301}"/>
+    <hyperlink ref="C490" r:id="rId447" xr:uid="{19A7BFB1-FE69-485C-B01A-3D0FC3768D75}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId447"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId448"/>
 </worksheet>
 </file>
</xml_diff>